<commit_message>
Añadi Preguntas al excel
Falta Hacer cambios en el codigo
</commit_message>
<xml_diff>
--- a/Archivo Exel/PInt.xlsx
+++ b/Archivo Exel/PInt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sergiogonzalez/Documents/GitHub/ProyectoIntegradorPrimerSemestre/Archivo Exel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA1012F2-504D-FE47-89AF-1FEFBF331C2E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{058245C2-8C3B-CA4D-AD8E-CB5D164D1502}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3900" yWindow="2260" windowWidth="28040" windowHeight="17440" xr2:uid="{F4C8BBAB-4DFE-1142-B99E-3F27D2E75C10}"/>
   </bookViews>
@@ -33,27 +33,99 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>Nombres</t>
-  </si>
-  <si>
-    <t>Edades</t>
-  </si>
-  <si>
-    <t>Juan</t>
-  </si>
-  <si>
-    <t>Jose</t>
-  </si>
-  <si>
-    <t>Santiag</t>
-  </si>
-  <si>
-    <t>Fernanda</t>
-  </si>
-  <si>
-    <t>Petronila</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="31">
+  <si>
+    <t>Preguntas</t>
+  </si>
+  <si>
+    <t>Res_C</t>
+  </si>
+  <si>
+    <t>Res_I_1</t>
+  </si>
+  <si>
+    <t>Res_I_2</t>
+  </si>
+  <si>
+    <t>a)</t>
+  </si>
+  <si>
+    <t>b)</t>
+  </si>
+  <si>
+    <t>c)</t>
+  </si>
+  <si>
+    <t>¿Cómo se llama el componente mínimo que forma a los seres vivos?</t>
+  </si>
+  <si>
+    <t>Célula</t>
+  </si>
+  <si>
+    <t>Partícula</t>
+  </si>
+  <si>
+    <t>Tejido</t>
+  </si>
+  <si>
+    <t>El proceso por el que una célula se divide para formar dos células hijas se llama:</t>
+  </si>
+  <si>
+    <t>Mitosis</t>
+  </si>
+  <si>
+    <t>Meiosis</t>
+  </si>
+  <si>
+    <t>Segregación</t>
+  </si>
+  <si>
+    <t>La información genética en las células se localiza:</t>
+  </si>
+  <si>
+    <t>El Nucleo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">En la membrana </t>
+  </si>
+  <si>
+    <t>En el Citoplasma</t>
+  </si>
+  <si>
+    <t>¿Con qué respira una ballena?</t>
+  </si>
+  <si>
+    <t>Pulmones</t>
+  </si>
+  <si>
+    <t>Por la piel</t>
+  </si>
+  <si>
+    <t>Branquias</t>
+  </si>
+  <si>
+    <t>Los cromosomas están formados por:</t>
+  </si>
+  <si>
+    <t>ADN</t>
+  </si>
+  <si>
+    <t>Proteinas</t>
+  </si>
+  <si>
+    <t>ARN</t>
+  </si>
+  <si>
+    <t>Al descendiente del cruce de un asno y una yegua se le conoce como:</t>
+  </si>
+  <si>
+    <t>Mula</t>
+  </si>
+  <si>
+    <t>Burro</t>
+  </si>
+  <si>
+    <t>Asno</t>
   </si>
 </sst>
 </file>
@@ -89,8 +161,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -405,61 +483,373 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F848DBF8-B63A-404E-86A0-789AE27EEDD7}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21.6640625" customWidth="1"/>
+    <col min="2" max="2" width="6.5" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="C1" s="1"/>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2">
+      <c r="E1" s="1"/>
+      <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+    </row>
+    <row r="2" spans="1:9" ht="68" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+    </row>
+    <row r="3" spans="1:9" ht="68" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3">
+      <c r="F3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+    </row>
+    <row r="4" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="C4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B5">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="E4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B6">
-        <v>11</v>
-      </c>
+      <c r="G4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+    </row>
+    <row r="6" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="1:9" ht="68" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
1/4 Del quizz completo
</commit_message>
<xml_diff>
--- a/Archivo Exel/PInt.xlsx
+++ b/Archivo Exel/PInt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sergiogonzalez/Documents/GitHub/ProyectoIntegradorPrimerSemestre/Archivo Exel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{058245C2-8C3B-CA4D-AD8E-CB5D164D1502}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2D75D12-E471-EF42-9699-438BD64EE57C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3900" yWindow="2260" windowWidth="28040" windowHeight="17440" xr2:uid="{F4C8BBAB-4DFE-1142-B99E-3F27D2E75C10}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="34">
   <si>
     <t>Preguntas</t>
   </si>
@@ -126,6 +126,15 @@
   </si>
   <si>
     <t>Asno</t>
+  </si>
+  <si>
+    <t>Res_CC</t>
+  </si>
+  <si>
+    <t>Res_II_1</t>
+  </si>
+  <si>
+    <t>Res_II_2</t>
   </si>
 </sst>
 </file>
@@ -486,7 +495,7 @@
   <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -502,15 +511,21 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1"/>
+      <c r="C1" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1"/>
+      <c r="E1" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="1"/>
+      <c r="G1" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
     </row>

</xml_diff>

<commit_message>
update main y lecturas
</commit_message>
<xml_diff>
--- a/Archivo Exel/PInt.xlsx
+++ b/Archivo Exel/PInt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sergiogonzalez/Documents/GitHub/ProyectoIntegradorPrimerSemestre/Archivo Exel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A983D47D-1DB5-624A-9FA8-65C2067C192D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F9E0790-FBF7-C848-98C0-8F40A58A2C93}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17920" windowHeight="22400" xr2:uid="{F4C8BBAB-4DFE-1142-B99E-3F27D2E75C10}"/>
   </bookViews>
@@ -550,7 +550,7 @@
   <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>